<commit_message>
Hotfix: update demo project framework and progbook
Converted annual probabilities to daily probabilities for diagnosis and
treatment
</commit_message>
<xml_diff>
--- a/atomica_apps/optima_tb_framework.xlsx
+++ b/atomica_apps/optima_tb_framework.xlsx
@@ -4437,43 +4437,7 @@
     <t>nx_nnotif*(1-nx_prop_ep)/max(nx_prop_notif, 1e-15)</t>
   </si>
   <si>
-    <t>pd_ndiag/max(spdu, 1e-15)</t>
-  </si>
-  <si>
-    <t>pm_ndiag/max(spmu, 1e-15)</t>
-  </si>
-  <si>
-    <t>px_ndiag/max(spxu, 1e-15)</t>
-  </si>
-  <si>
-    <t>nd_ndiag/max(sndu, 1e-15)</t>
-  </si>
-  <si>
-    <t>nm_ndiag/max(snmu, 1e-15)</t>
-  </si>
-  <si>
-    <t>nx_ndiag/max(snxu, 1e-15)</t>
-  </si>
-  <si>
     <t>Timescale</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SP-DS</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SP-MDR</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SP-XDR</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SN-DS</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SN-MDR</t>
-  </si>
-  <si>
-    <t>Annual diagnosis probability for SN-XDR</t>
   </si>
   <si>
     <t>ac_incidence_epc</t>
@@ -5313,24 +5277,6 @@
     <t>x_prob_treat</t>
   </si>
   <si>
-    <t>m_ntreat/max(spmd+snmd, 1e-15)</t>
-  </si>
-  <si>
-    <t>Annual treatment probability for diagnosed DS-TB</t>
-  </si>
-  <si>
-    <t>Annual treatment probability for diagnosed MDR-TB</t>
-  </si>
-  <si>
-    <t>Annual treatment probability for diagnosed XDR-TB</t>
-  </si>
-  <si>
-    <t>x_ntreat/max(spxd+snxd, 1e-15)</t>
-  </si>
-  <si>
-    <t>d_ntreat/max(spdd+sndd, 1e-15)</t>
-  </si>
-  <si>
     <t>Enter the total number of people in each population.
 The first value entered in the row will be used by the model to initialize the number of people alive in the first time step. For example if the model starts in year 2000 then the first value entered for each population would be used as the population size as of 1 Jan 2000.</t>
   </si>
@@ -5342,6 +5288,60 @@
   </si>
   <si>
     <t>{'Active XDR-TB treatment initiation':['x_prob_treat:flow']}</t>
+  </si>
+  <si>
+    <t>Daily treatment probability for diagnosed XDR-TB</t>
+  </si>
+  <si>
+    <t>Daily treatment probability for diagnosed MDR-TB</t>
+  </si>
+  <si>
+    <t>Daily treatment probability for diagnosed DS-TB</t>
+  </si>
+  <si>
+    <t>m_ntreat/max((spmd+snmd)*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>d_ntreat/max((spdd+sndd)*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>x_ntreat/max((spxd+snxd)*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>pd_ndiag/max(spdu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>pm_ndiag/max(spmu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>px_ndiag/max(spxu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>nd_ndiag/max(sndu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>nm_ndiag/max(snmu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>nx_ndiag/max(snxu*365, 1e-15)</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SP-DS</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SP-MDR</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SP-XDR</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SN-DS</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SN-MDR</t>
+  </si>
+  <si>
+    <t>Daily diagnosis probability for SN-XDR</t>
   </si>
 </sst>
 </file>
@@ -5635,28 +5635,7 @@
     <cellStyle name="Neutral 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -6138,7 +6117,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6324,7 +6303,7 @@
         <v>718</v>
       </c>
       <c r="C13" t="s">
-        <v>1216</v>
+        <v>1204</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>1012</v>
@@ -6422,7 +6401,7 @@
         <v>718</v>
       </c>
       <c r="C20" t="s">
-        <v>1210</v>
+        <v>1198</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>449</v>
@@ -6436,7 +6415,7 @@
         <v>718</v>
       </c>
       <c r="C21" t="s">
-        <v>1211</v>
+        <v>1199</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>449</v>
@@ -6450,7 +6429,7 @@
         <v>718</v>
       </c>
       <c r="C22" t="s">
-        <v>1212</v>
+        <v>1200</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>449</v>
@@ -6464,7 +6443,7 @@
         <v>718</v>
       </c>
       <c r="C23" t="s">
-        <v>1215</v>
+        <v>1203</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>449</v>
@@ -6478,7 +6457,7 @@
         <v>718</v>
       </c>
       <c r="C24" t="s">
-        <v>1213</v>
+        <v>1201</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>449</v>
@@ -6492,7 +6471,7 @@
         <v>718</v>
       </c>
       <c r="C25" t="s">
-        <v>1214</v>
+        <v>1202</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>449</v>
@@ -6506,7 +6485,7 @@
         <v>718</v>
       </c>
       <c r="C26" t="s">
-        <v>1372</v>
+        <v>1354</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>1025</v>
@@ -6520,7 +6499,7 @@
         <v>718</v>
       </c>
       <c r="C27" t="s">
-        <v>1373</v>
+        <v>1355</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>1025</v>
@@ -6534,7 +6513,7 @@
         <v>718</v>
       </c>
       <c r="C28" t="s">
-        <v>1374</v>
+        <v>1356</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>1025</v>
@@ -6542,13 +6521,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>1217</v>
+        <v>1205</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>718</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>1185</v>
+        <v>1173</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>1012</v>
@@ -6640,7 +6619,7 @@
         <v>1053</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1209</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6784,7 +6763,7 @@
         <v>1046</v>
       </c>
       <c r="K2" s="58" t="s">
-        <v>1371</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -7985,9 +7964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY51"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH22" sqref="AH22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8506,7 +8485,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="Q16" s="5" t="s">
-        <v>1194</v>
+        <v>1182</v>
       </c>
       <c r="AO16" s="5" t="s">
         <v>182</v>
@@ -8526,8 +8505,8 @@
         <v>66</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="R17" s="5" t="s">
-        <v>1362</v>
+      <c r="R17" s="27" t="s">
+        <v>1350</v>
       </c>
       <c r="AO17" s="5" t="s">
         <v>182</v>
@@ -8584,7 +8563,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="U20" s="5" t="s">
-        <v>1195</v>
+        <v>1183</v>
       </c>
       <c r="AO20" s="5" t="s">
         <v>191</v>
@@ -8605,7 +8584,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="V21" s="5" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="AO21" s="5" t="s">
         <v>191</v>
@@ -8664,7 +8643,7 @@
       <c r="B24" s="2"/>
       <c r="X24" s="8"/>
       <c r="Y24" s="5" t="s">
-        <v>1196</v>
+        <v>1184</v>
       </c>
       <c r="AO24" s="5" t="s">
         <v>200</v>
@@ -8685,7 +8664,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="Z25" s="5" t="s">
-        <v>1364</v>
+        <v>1352</v>
       </c>
       <c r="AO25" s="5" t="s">
         <v>200</v>
@@ -8755,7 +8734,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="AD29" s="5" t="s">
-        <v>1197</v>
+        <v>1185</v>
       </c>
       <c r="AO29" s="5" t="s">
         <v>211</v>
@@ -8776,7 +8755,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="AE30" s="5" t="s">
-        <v>1362</v>
+        <v>1350</v>
       </c>
       <c r="AO30" s="5" t="s">
         <v>211</v>
@@ -8834,7 +8813,7 @@
       </c>
       <c r="B33" s="2"/>
       <c r="AH33" s="5" t="s">
-        <v>1198</v>
+        <v>1186</v>
       </c>
       <c r="AO33" s="5" t="s">
         <v>219</v>
@@ -8855,7 +8834,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="AI34" s="5" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="AO34" s="5" t="s">
         <v>219</v>
@@ -8913,7 +8892,7 @@
       </c>
       <c r="B37" s="2"/>
       <c r="AL37" s="5" t="s">
-        <v>1199</v>
+        <v>1187</v>
       </c>
       <c r="AO37" s="5" t="s">
         <v>227</v>
@@ -8934,7 +8913,7 @@
       </c>
       <c r="B38" s="2"/>
       <c r="AM38" s="5" t="s">
-        <v>1364</v>
+        <v>1352</v>
       </c>
       <c r="AO38" s="5" t="s">
         <v>227</v>
@@ -9078,8 +9057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9156,7 +9135,7 @@
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="21" t="s">
-        <v>1301</v>
+        <v>1289</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -9182,7 +9161,7 @@
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="21" t="s">
-        <v>1302</v>
+        <v>1290</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -9208,7 +9187,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="21" t="s">
-        <v>1303</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
@@ -9233,7 +9212,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="21" t="s">
-        <v>1304</v>
+        <v>1292</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -9259,7 +9238,7 @@
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="21" t="s">
-        <v>1305</v>
+        <v>1293</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -9285,7 +9264,7 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="21" t="s">
-        <v>1306</v>
+        <v>1294</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -9311,7 +9290,7 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="21" t="s">
-        <v>1307</v>
+        <v>1295</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="3"/>
@@ -9338,7 +9317,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="21" t="s">
-        <v>1308</v>
+        <v>1296</v>
       </c>
       <c r="K9" s="14"/>
       <c r="L9" s="3"/>
@@ -9365,7 +9344,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="21" t="s">
-        <v>1309</v>
+        <v>1297</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="3"/>
@@ -9392,7 +9371,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="21" t="s">
-        <v>1310</v>
+        <v>1298</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="3"/>
@@ -9419,7 +9398,7 @@
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="21" t="s">
-        <v>1311</v>
+        <v>1299</v>
       </c>
       <c r="K12" s="14"/>
       <c r="L12" s="3"/>
@@ -9446,7 +9425,7 @@
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="21" t="s">
-        <v>1312</v>
+        <v>1300</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="3"/>
@@ -9514,7 +9493,7 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="21" t="s">
-        <v>1313</v>
+        <v>1301</v>
       </c>
       <c r="K16" s="14"/>
       <c r="L16" s="3"/>
@@ -9541,7 +9520,7 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="21" t="s">
-        <v>1314</v>
+        <v>1302</v>
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="3"/>
@@ -9568,7 +9547,7 @@
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="21" t="s">
-        <v>1315</v>
+        <v>1303</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="3"/>
@@ -9595,7 +9574,7 @@
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="21" t="s">
-        <v>1316</v>
+        <v>1304</v>
       </c>
       <c r="K19" s="14"/>
       <c r="L19" s="3"/>
@@ -9622,7 +9601,7 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="21" t="s">
-        <v>1317</v>
+        <v>1305</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="3"/>
@@ -9649,7 +9628,7 @@
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="21" t="s">
-        <v>1318</v>
+        <v>1306</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="3"/>
@@ -9676,7 +9655,7 @@
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="21" t="s">
-        <v>1319</v>
+        <v>1307</v>
       </c>
       <c r="K22" s="14"/>
     </row>
@@ -9702,7 +9681,7 @@
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="21" t="s">
-        <v>1320</v>
+        <v>1308</v>
       </c>
       <c r="K23" s="14"/>
     </row>
@@ -9804,7 +9783,7 @@
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="21" t="s">
-        <v>1321</v>
+        <v>1309</v>
       </c>
       <c r="K28" s="14"/>
     </row>
@@ -9849,7 +9828,7 @@
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="57" t="s">
-        <v>1361</v>
+        <v>1349</v>
       </c>
       <c r="K30" s="14"/>
     </row>
@@ -10458,7 +10437,7 @@
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="21" t="s">
-        <v>1322</v>
+        <v>1310</v>
       </c>
       <c r="K57" s="14"/>
       <c r="L57" s="3"/>
@@ -10485,7 +10464,7 @@
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="21" t="s">
-        <v>1323</v>
+        <v>1311</v>
       </c>
       <c r="K58" s="14"/>
       <c r="L58" s="3"/>
@@ -10512,7 +10491,7 @@
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="21" t="s">
-        <v>1324</v>
+        <v>1312</v>
       </c>
       <c r="K59" s="14"/>
       <c r="L59" s="3"/>
@@ -10539,7 +10518,7 @@
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="21" t="s">
-        <v>1325</v>
+        <v>1313</v>
       </c>
       <c r="K60" s="14"/>
       <c r="L60" s="3"/>
@@ -10623,7 +10602,7 @@
       </c>
       <c r="I64" s="5"/>
       <c r="J64" s="21" t="s">
-        <v>1326</v>
+        <v>1314</v>
       </c>
       <c r="K64" s="14"/>
       <c r="L64" s="3"/>
@@ -10650,7 +10629,7 @@
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="21" t="s">
-        <v>1352</v>
+        <v>1340</v>
       </c>
       <c r="K65" s="14"/>
       <c r="L65" s="3"/>
@@ -10677,7 +10656,7 @@
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="21" t="s">
-        <v>1327</v>
+        <v>1315</v>
       </c>
       <c r="K66" s="14"/>
       <c r="L66" s="3"/>
@@ -10725,7 +10704,7 @@
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="21" t="s">
-        <v>1328</v>
+        <v>1316</v>
       </c>
       <c r="K68" s="14"/>
     </row>
@@ -10889,17 +10868,17 @@
   <dimension ref="A1:O346"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C72" sqref="C72"/>
+      <selection pane="bottomRight" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -10927,7 +10906,7 @@
         <v>426</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>242</v>
@@ -10994,7 +10973,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>1344</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11028,7 +11007,7 @@
         <v>14</v>
       </c>
       <c r="O3" s="28" t="s">
-        <v>1345</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -11065,7 +11044,7 @@
         <v>14</v>
       </c>
       <c r="O4" s="28" t="s">
-        <v>1351</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="29" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -11102,7 +11081,7 @@
         <v>14</v>
       </c>
       <c r="O5" s="28" t="s">
-        <v>1346</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11138,7 +11117,7 @@
         <v>14</v>
       </c>
       <c r="O6" s="28" t="s">
-        <v>1347</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11174,7 +11153,7 @@
         <v>14</v>
       </c>
       <c r="O7" s="28" t="s">
-        <v>1348</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -11210,7 +11189,7 @@
         <v>14</v>
       </c>
       <c r="O8" s="28" t="s">
-        <v>1349</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -11246,7 +11225,7 @@
         <v>14</v>
       </c>
       <c r="O9" s="28" t="s">
-        <v>1350</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -11254,7 +11233,7 @@
         <v>176</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1218</v>
+        <v>1206</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>433</v>
@@ -11285,7 +11264,7 @@
       </c>
       <c r="N10" s="26"/>
       <c r="O10" s="21" t="s">
-        <v>1231</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -11293,7 +11272,7 @@
         <v>177</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1219</v>
+        <v>1207</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>433</v>
@@ -11324,7 +11303,7 @@
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="21" t="s">
-        <v>1230</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11332,7 +11311,7 @@
         <v>178</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1221</v>
+        <v>1209</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>433</v>
@@ -11363,7 +11342,7 @@
       </c>
       <c r="N12" s="26"/>
       <c r="O12" s="21" t="s">
-        <v>1229</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11371,7 +11350,7 @@
         <v>179</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1220</v>
+        <v>1208</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>433</v>
@@ -11402,7 +11381,7 @@
       </c>
       <c r="N13" s="26"/>
       <c r="O13" s="21" t="s">
-        <v>1353</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11410,7 +11389,7 @@
         <v>180</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1222</v>
+        <v>1210</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>433</v>
@@ -11441,7 +11420,7 @@
       </c>
       <c r="N14" s="26"/>
       <c r="O14" s="21" t="s">
-        <v>1228</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11449,7 +11428,7 @@
         <v>207</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1223</v>
+        <v>1211</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>433</v>
@@ -11480,7 +11459,7 @@
       </c>
       <c r="N15" s="26"/>
       <c r="O15" s="21" t="s">
-        <v>1227</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11488,7 +11467,7 @@
         <v>208</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1224</v>
+        <v>1212</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>433</v>
@@ -11519,7 +11498,7 @@
       </c>
       <c r="N16" s="26"/>
       <c r="O16" s="21" t="s">
-        <v>1358</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -11527,7 +11506,7 @@
         <v>209</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1225</v>
+        <v>1213</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>433</v>
@@ -11558,7 +11537,7 @@
       </c>
       <c r="N17" s="26"/>
       <c r="O17" s="21" t="s">
-        <v>1226</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -11595,7 +11574,7 @@
       </c>
       <c r="N18" s="26"/>
       <c r="O18" s="21" t="s">
-        <v>1359</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="120" x14ac:dyDescent="0.25">
@@ -11628,7 +11607,7 @@
       </c>
       <c r="N19" s="26"/>
       <c r="O19" s="21" t="s">
-        <v>1360</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -11661,7 +11640,7 @@
       </c>
       <c r="N20" s="26"/>
       <c r="O20" s="21" t="s">
-        <v>1232</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -11696,7 +11675,7 @@
       </c>
       <c r="N21" s="26"/>
       <c r="O21" s="21" t="s">
-        <v>1233</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -11729,7 +11708,7 @@
       </c>
       <c r="N22" s="26"/>
       <c r="O22" s="21" t="s">
-        <v>1234</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -11762,7 +11741,7 @@
       </c>
       <c r="N23" s="26"/>
       <c r="O23" s="21" t="s">
-        <v>1354</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -11795,7 +11774,7 @@
       </c>
       <c r="N24" s="26"/>
       <c r="O24" s="21" t="s">
-        <v>1235</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -12782,7 +12761,7 @@
       </c>
       <c r="N53" s="26"/>
       <c r="O53" s="21" t="s">
-        <v>1239</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -12817,7 +12796,7 @@
       </c>
       <c r="N54" s="26"/>
       <c r="O54" s="21" t="s">
-        <v>1236</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -12854,7 +12833,7 @@
       </c>
       <c r="N55" s="26"/>
       <c r="O55" s="21" t="s">
-        <v>1237</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -12891,7 +12870,7 @@
       </c>
       <c r="N56" s="26"/>
       <c r="O56" s="21" t="s">
-        <v>1238</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -12925,7 +12904,7 @@
       </c>
       <c r="N57" s="26"/>
       <c r="O57" s="21" t="s">
-        <v>1240</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -12961,7 +12940,7 @@
       </c>
       <c r="N58" s="26"/>
       <c r="O58" s="21" t="s">
-        <v>1241</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -12997,7 +12976,7 @@
       </c>
       <c r="N59" s="26"/>
       <c r="O59" s="21" t="s">
-        <v>1242</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -13030,7 +13009,7 @@
       </c>
       <c r="N60" s="26"/>
       <c r="O60" s="21" t="s">
-        <v>1243</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -13065,7 +13044,7 @@
       </c>
       <c r="N61" s="26"/>
       <c r="O61" s="21" t="s">
-        <v>1244</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -13100,7 +13079,7 @@
       </c>
       <c r="N62" s="26"/>
       <c r="O62" s="21" t="s">
-        <v>1245</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -13383,7 +13362,7 @@
       </c>
       <c r="N71" s="26"/>
       <c r="O71" s="21" t="s">
-        <v>1246</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -13422,7 +13401,7 @@
       </c>
       <c r="N72" s="26"/>
       <c r="O72" s="21" t="s">
-        <v>1247</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -13459,7 +13438,7 @@
       </c>
       <c r="N73" s="26"/>
       <c r="O73" s="21" t="s">
-        <v>1248</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -14039,7 +14018,7 @@
       </c>
       <c r="N92" s="26"/>
       <c r="O92" s="21" t="s">
-        <v>1249</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -14074,7 +14053,7 @@
       </c>
       <c r="N93" s="26"/>
       <c r="O93" s="21" t="s">
-        <v>1250</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="94" spans="1:15" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -14109,7 +14088,7 @@
       </c>
       <c r="N94" s="31"/>
       <c r="O94" s="21" t="s">
-        <v>1251</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="95" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -14209,7 +14188,7 @@
       </c>
       <c r="N97" s="31"/>
       <c r="O97" s="21" t="s">
-        <v>1252</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="98" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -14275,7 +14254,7 @@
       </c>
       <c r="N99" s="27"/>
       <c r="O99" s="28" t="s">
-        <v>1253</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="100" spans="1:15" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14308,7 +14287,7 @@
       </c>
       <c r="N100" s="27"/>
       <c r="O100" s="28" t="s">
-        <v>1355</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="101" spans="1:15" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14341,7 +14320,7 @@
       </c>
       <c r="N101" s="27"/>
       <c r="O101" s="28" t="s">
-        <v>1254</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="102" spans="1:15" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14374,7 +14353,7 @@
       </c>
       <c r="N102" s="27"/>
       <c r="O102" s="28" t="s">
-        <v>1255</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="103" spans="1:15" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14407,7 +14386,7 @@
       </c>
       <c r="N103" s="27"/>
       <c r="O103" s="28" t="s">
-        <v>1356</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="104" spans="1:15" s="29" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -14440,7 +14419,7 @@
       </c>
       <c r="N104" s="27"/>
       <c r="O104" s="28" t="s">
-        <v>1256</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="105" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14475,7 +14454,7 @@
       </c>
       <c r="N105" s="27"/>
       <c r="O105" s="28" t="s">
-        <v>1257</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="106" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14510,7 +14489,7 @@
       </c>
       <c r="N106" s="27"/>
       <c r="O106" s="28" t="s">
-        <v>1258</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="107" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14545,7 +14524,7 @@
       </c>
       <c r="N107" s="27"/>
       <c r="O107" s="28" t="s">
-        <v>1259</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="108" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14580,7 +14559,7 @@
       </c>
       <c r="N108" s="27"/>
       <c r="O108" s="28" t="s">
-        <v>1260</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="109" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14615,7 +14594,7 @@
       </c>
       <c r="N109" s="27"/>
       <c r="O109" s="28" t="s">
-        <v>1261</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="110" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -14650,7 +14629,7 @@
       </c>
       <c r="N110" s="27"/>
       <c r="O110" s="28" t="s">
-        <v>1262</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="111" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14685,7 +14664,7 @@
       </c>
       <c r="N111" s="27"/>
       <c r="O111" s="28" t="s">
-        <v>1263</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="112" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14720,7 +14699,7 @@
       </c>
       <c r="N112" s="27"/>
       <c r="O112" s="28" t="s">
-        <v>1264</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="113" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14755,7 +14734,7 @@
       </c>
       <c r="N113" s="27"/>
       <c r="O113" s="28" t="s">
-        <v>1265</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="114" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14790,7 +14769,7 @@
       </c>
       <c r="N114" s="27"/>
       <c r="O114" s="28" t="s">
-        <v>1266</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="115" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14825,7 +14804,7 @@
       </c>
       <c r="N115" s="27"/>
       <c r="O115" s="28" t="s">
-        <v>1267</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="116" spans="1:15" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -14860,7 +14839,7 @@
       </c>
       <c r="N116" s="27"/>
       <c r="O116" s="28" t="s">
-        <v>1268</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="117" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -15051,24 +15030,27 @@
     </row>
     <row r="123" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="42" t="s">
-        <v>1194</v>
+        <v>1182</v>
       </c>
       <c r="B123" s="43" t="s">
-        <v>1164</v>
+        <v>1369</v>
       </c>
       <c r="C123" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D123" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E123" s="42"/>
       <c r="F123" s="42">
         <v>0</v>
       </c>
-      <c r="G123" s="42"/>
+      <c r="G123" s="42">
+        <v>1</v>
+      </c>
       <c r="H123" s="42" t="s">
-        <v>1157</v>
+        <v>1363</v>
       </c>
       <c r="I123" s="44" t="s">
         <v>1046</v>
@@ -15085,24 +15067,27 @@
     </row>
     <row r="124" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="42" t="s">
-        <v>1195</v>
+        <v>1183</v>
       </c>
       <c r="B124" s="43" t="s">
-        <v>1165</v>
+        <v>1370</v>
       </c>
       <c r="C124" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D124" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E124" s="42"/>
       <c r="F124" s="42">
         <v>0</v>
       </c>
-      <c r="G124" s="42"/>
+      <c r="G124" s="42">
+        <v>1</v>
+      </c>
       <c r="H124" s="42" t="s">
-        <v>1158</v>
+        <v>1364</v>
       </c>
       <c r="I124" s="44" t="s">
         <v>1046</v>
@@ -15119,24 +15104,27 @@
     </row>
     <row r="125" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="42" t="s">
-        <v>1196</v>
+        <v>1184</v>
       </c>
       <c r="B125" s="43" t="s">
-        <v>1166</v>
+        <v>1371</v>
       </c>
       <c r="C125" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D125" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E125" s="42"/>
       <c r="F125" s="42">
         <v>0</v>
       </c>
-      <c r="G125" s="42"/>
+      <c r="G125" s="42">
+        <v>1</v>
+      </c>
       <c r="H125" s="42" t="s">
-        <v>1159</v>
+        <v>1365</v>
       </c>
       <c r="I125" s="44" t="s">
         <v>1046</v>
@@ -15153,24 +15141,27 @@
     </row>
     <row r="126" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="42" t="s">
-        <v>1197</v>
+        <v>1185</v>
       </c>
       <c r="B126" s="43" t="s">
-        <v>1167</v>
+        <v>1372</v>
       </c>
       <c r="C126" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D126" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E126" s="42"/>
       <c r="F126" s="42">
         <v>0</v>
       </c>
-      <c r="G126" s="42"/>
+      <c r="G126" s="42">
+        <v>1</v>
+      </c>
       <c r="H126" s="42" t="s">
-        <v>1160</v>
+        <v>1366</v>
       </c>
       <c r="I126" s="44" t="s">
         <v>1046</v>
@@ -15187,24 +15178,27 @@
     </row>
     <row r="127" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="42" t="s">
-        <v>1198</v>
+        <v>1186</v>
       </c>
       <c r="B127" s="43" t="s">
-        <v>1168</v>
+        <v>1373</v>
       </c>
       <c r="C127" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D127" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E127" s="42"/>
       <c r="F127" s="42">
         <v>0</v>
       </c>
-      <c r="G127" s="42"/>
+      <c r="G127" s="42">
+        <v>1</v>
+      </c>
       <c r="H127" s="42" t="s">
-        <v>1161</v>
+        <v>1367</v>
       </c>
       <c r="I127" s="44" t="s">
         <v>1046</v>
@@ -15221,24 +15215,27 @@
     </row>
     <row r="128" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="42" t="s">
-        <v>1199</v>
+        <v>1187</v>
       </c>
       <c r="B128" s="43" t="s">
-        <v>1169</v>
+        <v>1374</v>
       </c>
       <c r="C128" s="42" t="s">
         <v>523</v>
       </c>
       <c r="D128" s="42">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E128" s="42"/>
       <c r="F128" s="42">
         <v>0</v>
       </c>
-      <c r="G128" s="42"/>
+      <c r="G128" s="42">
+        <v>1</v>
+      </c>
       <c r="H128" s="42" t="s">
-        <v>1162</v>
+        <v>1368</v>
       </c>
       <c r="I128" s="44" t="s">
         <v>1046</v>
@@ -15282,21 +15279,22 @@
       </c>
       <c r="N129" s="27"/>
       <c r="O129" s="28" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="130" spans="1:15" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27" t="s">
-        <v>1362</v>
+        <v>1350</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>1366</v>
+        <v>1359</v>
       </c>
       <c r="C130" s="27" t="s">
         <v>523</v>
       </c>
       <c r="D130" s="27">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E130" s="27"/>
       <c r="F130" s="27">
@@ -15306,7 +15304,7 @@
         <v>1</v>
       </c>
       <c r="H130" s="27" t="s">
-        <v>1370</v>
+        <v>1361</v>
       </c>
       <c r="I130" s="30" t="s">
         <v>1046</v>
@@ -15356,7 +15354,7 @@
       </c>
       <c r="N131" s="27"/>
       <c r="O131" s="28" t="s">
-        <v>1271</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="132" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -15395,7 +15393,7 @@
       </c>
       <c r="N132" s="27"/>
       <c r="O132" s="28" t="s">
-        <v>1272</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="133" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -15434,7 +15432,7 @@
       </c>
       <c r="N133" s="27"/>
       <c r="O133" s="28" t="s">
-        <v>1273</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="134" spans="1:15" s="29" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -15473,7 +15471,7 @@
       </c>
       <c r="N134" s="27"/>
       <c r="O134" s="28" t="s">
-        <v>1274</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="135" spans="1:15" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -15512,7 +15510,7 @@
       </c>
       <c r="N135" s="27"/>
       <c r="O135" s="28" t="s">
-        <v>1275</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="136" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -15551,7 +15549,7 @@
       </c>
       <c r="N136" s="27"/>
       <c r="O136" s="28" t="s">
-        <v>1276</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="137" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -15943,21 +15941,22 @@
       </c>
       <c r="N148" s="27"/>
       <c r="O148" s="28" t="s">
-        <v>1357</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="149" spans="1:15" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="27" t="s">
-        <v>1363</v>
+        <v>1351</v>
       </c>
       <c r="B149" s="28" t="s">
-        <v>1367</v>
+        <v>1358</v>
       </c>
       <c r="C149" s="27" t="s">
         <v>523</v>
       </c>
       <c r="D149" s="27">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E149" s="27"/>
       <c r="F149" s="27">
@@ -15967,7 +15966,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="27" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="I149" s="30" t="s">
         <v>1046</v>
@@ -16017,7 +16016,7 @@
       </c>
       <c r="N150" s="27"/>
       <c r="O150" s="28" t="s">
-        <v>1282</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="151" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -16056,7 +16055,7 @@
       </c>
       <c r="N151" s="27"/>
       <c r="O151" s="28" t="s">
-        <v>1287</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="152" spans="1:15" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -16095,7 +16094,7 @@
       </c>
       <c r="N152" s="27"/>
       <c r="O152" s="28" t="s">
-        <v>1286</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="153" spans="1:15" s="29" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -16134,7 +16133,7 @@
       </c>
       <c r="N153" s="27"/>
       <c r="O153" s="28" t="s">
-        <v>1285</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="154" spans="1:15" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -16173,7 +16172,7 @@
       </c>
       <c r="N154" s="27"/>
       <c r="O154" s="28" t="s">
-        <v>1284</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="155" spans="1:15" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -16212,7 +16211,7 @@
       </c>
       <c r="N155" s="27"/>
       <c r="O155" s="28" t="s">
-        <v>1283</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="156" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -16604,21 +16603,22 @@
       </c>
       <c r="N167" s="49"/>
       <c r="O167" s="28" t="s">
-        <v>1270</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="168" spans="1:15" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="27" t="s">
-        <v>1364</v>
+        <v>1352</v>
       </c>
       <c r="B168" s="28" t="s">
-        <v>1368</v>
+        <v>1357</v>
       </c>
       <c r="C168" s="27" t="s">
         <v>523</v>
       </c>
       <c r="D168" s="27">
-        <v>1</v>
+        <f>1/365</f>
+        <v>2.7397260273972603E-3</v>
       </c>
       <c r="E168" s="27"/>
       <c r="F168" s="27">
@@ -16628,7 +16628,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="27" t="s">
-        <v>1369</v>
+        <v>1362</v>
       </c>
       <c r="I168" s="30" t="s">
         <v>1046</v>
@@ -16678,7 +16678,7 @@
       </c>
       <c r="N169" s="49"/>
       <c r="O169" s="28" t="s">
-        <v>1277</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="170" spans="1:15" s="51" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -16717,7 +16717,7 @@
       </c>
       <c r="N170" s="49"/>
       <c r="O170" s="28" t="s">
-        <v>1278</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="171" spans="1:15" s="51" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -16756,7 +16756,7 @@
       </c>
       <c r="N171" s="49"/>
       <c r="O171" s="28" t="s">
-        <v>1279</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="172" spans="1:15" s="51" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -16795,7 +16795,7 @@
       </c>
       <c r="N172" s="49"/>
       <c r="O172" s="28" t="s">
-        <v>1280</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="173" spans="1:15" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -16834,7 +16834,7 @@
       </c>
       <c r="N173" s="49"/>
       <c r="O173" s="28" t="s">
-        <v>1281</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="174" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -17163,7 +17163,7 @@
       </c>
       <c r="N183" s="26"/>
       <c r="O183" s="21" t="s">
-        <v>1292</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="184" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17198,7 +17198,7 @@
       </c>
       <c r="N184" s="26"/>
       <c r="O184" s="21" t="s">
-        <v>1291</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="185" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17233,7 +17233,7 @@
       </c>
       <c r="N185" s="26"/>
       <c r="O185" s="21" t="s">
-        <v>1290</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="186" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17268,7 +17268,7 @@
       </c>
       <c r="N186" s="26"/>
       <c r="O186" s="21" t="s">
-        <v>1289</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="187" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17303,7 +17303,7 @@
       </c>
       <c r="N187" s="26"/>
       <c r="O187" s="21" t="s">
-        <v>1288</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="188" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17338,7 +17338,7 @@
       </c>
       <c r="N188" s="26"/>
       <c r="O188" s="21" t="s">
-        <v>1288</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="189" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17373,7 +17373,7 @@
       </c>
       <c r="N189" s="26"/>
       <c r="O189" s="21" t="s">
-        <v>1293</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="190" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17408,7 +17408,7 @@
       </c>
       <c r="N190" s="26"/>
       <c r="O190" s="21" t="s">
-        <v>1294</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="191" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17443,7 +17443,7 @@
       </c>
       <c r="N191" s="26"/>
       <c r="O191" s="21" t="s">
-        <v>1295</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="192" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17478,7 +17478,7 @@
       </c>
       <c r="N192" s="26"/>
       <c r="O192" s="21" t="s">
-        <v>1296</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="193" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17513,7 +17513,7 @@
       </c>
       <c r="N193" s="26"/>
       <c r="O193" s="21" t="s">
-        <v>1297</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="194" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -17548,7 +17548,7 @@
       </c>
       <c r="N194" s="26"/>
       <c r="O194" s="21" t="s">
-        <v>1298</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.25">
@@ -17581,7 +17581,7 @@
         <v>747</v>
       </c>
       <c r="O196" s="21" t="s">
-        <v>1300</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.25">
@@ -17631,7 +17631,7 @@
         <v>747</v>
       </c>
       <c r="O198" s="21" t="s">
-        <v>1299</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.25">
@@ -17701,7 +17701,7 @@
         <v>1053</v>
       </c>
       <c r="O202" s="21" t="s">
-        <v>1329</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="203" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -17730,7 +17730,7 @@
         <v>1053</v>
       </c>
       <c r="O203" s="21" t="s">
-        <v>1329</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="204" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -17759,7 +17759,7 @@
         <v>1053</v>
       </c>
       <c r="O204" s="21" t="s">
-        <v>1329</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="205" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17788,7 +17788,7 @@
         <v>1053</v>
       </c>
       <c r="O205" s="21" t="s">
-        <v>1330</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="206" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17817,7 +17817,7 @@
         <v>1053</v>
       </c>
       <c r="O206" s="21" t="s">
-        <v>1330</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="207" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17846,7 +17846,7 @@
         <v>1053</v>
       </c>
       <c r="O207" s="21" t="s">
-        <v>1330</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="208" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17875,7 +17875,7 @@
         <v>1053</v>
       </c>
       <c r="O208" s="21" t="s">
-        <v>1331</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="209" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17904,7 +17904,7 @@
         <v>1053</v>
       </c>
       <c r="O209" s="21" t="s">
-        <v>1331</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="210" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -17933,7 +17933,7 @@
         <v>1053</v>
       </c>
       <c r="O210" s="21" t="s">
-        <v>1331</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="211" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -17962,7 +17962,7 @@
         <v>1053</v>
       </c>
       <c r="O211" s="21" t="s">
-        <v>1332</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="212" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -17991,7 +17991,7 @@
         <v>1053</v>
       </c>
       <c r="O212" s="21" t="s">
-        <v>1332</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="213" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -18020,7 +18020,7 @@
         <v>1053</v>
       </c>
       <c r="O213" s="21" t="s">
-        <v>1332</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="214" spans="1:15" x14ac:dyDescent="0.25">
@@ -18037,7 +18037,7 @@
       <c r="E214" s="26"/>
       <c r="G214" s="26"/>
       <c r="H214" s="6" t="s">
-        <v>1200</v>
+        <v>1188</v>
       </c>
       <c r="I214" s="30" t="s">
         <v>1046</v>
@@ -18145,7 +18145,7 @@
         <v>1053</v>
       </c>
       <c r="O219" s="21" t="s">
-        <v>1333</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="220" spans="1:15" x14ac:dyDescent="0.25">
@@ -19864,7 +19864,7 @@
         <v>18</v>
       </c>
       <c r="O316" s="21" t="s">
-        <v>1334</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="318" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -19891,7 +19891,7 @@
         <v>1053</v>
       </c>
       <c r="O318" s="21" t="s">
-        <v>1335</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="319" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -19919,7 +19919,7 @@
         <v>1053</v>
       </c>
       <c r="O319" s="21" t="s">
-        <v>1336</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="320" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -19947,7 +19947,7 @@
         <v>1053</v>
       </c>
       <c r="O320" s="21" t="s">
-        <v>1337</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="321" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -19975,7 +19975,7 @@
         <v>1053</v>
       </c>
       <c r="O321" s="21" t="s">
-        <v>1338</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="322" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -20003,7 +20003,7 @@
         <v>1053</v>
       </c>
       <c r="O322" s="21" t="s">
-        <v>1339</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="323" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -20031,7 +20031,7 @@
         <v>1053</v>
       </c>
       <c r="O323" s="21" t="s">
-        <v>1340</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="324" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -20058,7 +20058,7 @@
         <v>1053</v>
       </c>
       <c r="O324" s="21" t="s">
-        <v>1340</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="325" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -20085,7 +20085,7 @@
         <v>1053</v>
       </c>
       <c r="O325" s="21" t="s">
-        <v>1341</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="326" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -20112,7 +20112,7 @@
         <v>1053</v>
       </c>
       <c r="O326" s="21" t="s">
-        <v>1342</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="328" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -20139,15 +20139,15 @@
         <v>18</v>
       </c>
       <c r="O328" s="21" t="s">
-        <v>1343</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="330" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A330" s="56" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
       <c r="B330" s="28" t="s">
-        <v>1188</v>
+        <v>1176</v>
       </c>
       <c r="C330" s="27" t="s">
         <v>521</v>
@@ -20161,7 +20161,7 @@
       </c>
       <c r="G330" s="27"/>
       <c r="H330" s="27" t="s">
-        <v>1201</v>
+        <v>1189</v>
       </c>
       <c r="I330" s="6" t="s">
         <v>1046</v>
@@ -20169,10 +20169,10 @@
     </row>
     <row r="331" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A331" s="56" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B331" s="28" t="s">
         <v>1177</v>
-      </c>
-      <c r="B331" s="28" t="s">
-        <v>1189</v>
       </c>
       <c r="C331" s="27" t="s">
         <v>521</v>
@@ -20186,7 +20186,7 @@
       </c>
       <c r="G331" s="27"/>
       <c r="H331" s="27" t="s">
-        <v>1202</v>
+        <v>1190</v>
       </c>
       <c r="I331" s="6" t="s">
         <v>1046</v>
@@ -20194,10 +20194,10 @@
     </row>
     <row r="332" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A332" s="56" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B332" s="28" t="s">
         <v>1178</v>
-      </c>
-      <c r="B332" s="28" t="s">
-        <v>1190</v>
       </c>
       <c r="C332" s="27" t="s">
         <v>521</v>
@@ -20211,7 +20211,7 @@
       </c>
       <c r="G332" s="27"/>
       <c r="H332" s="27" t="s">
-        <v>1203</v>
+        <v>1191</v>
       </c>
       <c r="I332" s="6" t="s">
         <v>1046</v>
@@ -20219,10 +20219,10 @@
     </row>
     <row r="333" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A333" s="56" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B333" s="28" t="s">
         <v>1179</v>
-      </c>
-      <c r="B333" s="28" t="s">
-        <v>1191</v>
       </c>
       <c r="C333" s="27" t="s">
         <v>521</v>
@@ -20236,7 +20236,7 @@
       </c>
       <c r="G333" s="27"/>
       <c r="H333" s="27" t="s">
-        <v>1204</v>
+        <v>1192</v>
       </c>
       <c r="I333" s="6" t="s">
         <v>1046</v>
@@ -20244,10 +20244,10 @@
     </row>
     <row r="334" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A334" s="56" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B334" s="28" t="s">
         <v>1180</v>
-      </c>
-      <c r="B334" s="28" t="s">
-        <v>1192</v>
       </c>
       <c r="C334" s="27" t="s">
         <v>521</v>
@@ -20261,7 +20261,7 @@
       </c>
       <c r="G334" s="27"/>
       <c r="H334" s="27" t="s">
-        <v>1205</v>
+        <v>1193</v>
       </c>
       <c r="I334" s="6" t="s">
         <v>1046</v>
@@ -20269,10 +20269,10 @@
     </row>
     <row r="335" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A335" s="56" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B335" s="28" t="s">
         <v>1181</v>
-      </c>
-      <c r="B335" s="28" t="s">
-        <v>1193</v>
       </c>
       <c r="C335" s="27" t="s">
         <v>521</v>
@@ -20286,7 +20286,7 @@
       </c>
       <c r="G335" s="27"/>
       <c r="H335" s="27" t="s">
-        <v>1206</v>
+        <v>1194</v>
       </c>
       <c r="I335" s="6" t="s">
         <v>1046</v>
@@ -20294,10 +20294,10 @@
     </row>
     <row r="336" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
-        <v>1186</v>
+        <v>1174</v>
       </c>
       <c r="B336" s="32" t="s">
-        <v>1187</v>
+        <v>1175</v>
       </c>
       <c r="C336" s="26" t="s">
         <v>521</v>
@@ -20307,7 +20307,7 @@
         <v>0</v>
       </c>
       <c r="H336" s="6" t="s">
-        <v>1176</v>
+        <v>1164</v>
       </c>
       <c r="I336" s="6" t="s">
         <v>1046</v>
@@ -20315,10 +20315,10 @@
     </row>
     <row r="338" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
-        <v>1170</v>
+        <v>1158</v>
       </c>
       <c r="B338" s="32" t="s">
-        <v>1173</v>
+        <v>1161</v>
       </c>
       <c r="C338" s="26" t="s">
         <v>521</v>
@@ -20327,7 +20327,7 @@
         <v>0</v>
       </c>
       <c r="H338" s="6" t="s">
-        <v>1183</v>
+        <v>1171</v>
       </c>
       <c r="I338" s="30" t="s">
         <v>1046</v>
@@ -20335,10 +20335,10 @@
     </row>
     <row r="339" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
-        <v>1171</v>
+        <v>1159</v>
       </c>
       <c r="B339" s="32" t="s">
-        <v>1174</v>
+        <v>1162</v>
       </c>
       <c r="C339" s="26" t="s">
         <v>521</v>
@@ -20347,7 +20347,7 @@
         <v>0</v>
       </c>
       <c r="H339" s="6" t="s">
-        <v>1182</v>
+        <v>1170</v>
       </c>
       <c r="I339" s="30" t="s">
         <v>1046</v>
@@ -20355,10 +20355,10 @@
     </row>
     <row r="340" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
-        <v>1172</v>
+        <v>1160</v>
       </c>
       <c r="B340" s="32" t="s">
-        <v>1207</v>
+        <v>1195</v>
       </c>
       <c r="C340" s="26" t="s">
         <v>521</v>
@@ -20369,7 +20369,7 @@
         <v>0</v>
       </c>
       <c r="H340" s="6" t="s">
-        <v>1184</v>
+        <v>1172</v>
       </c>
       <c r="I340" s="30" t="s">
         <v>1046</v>
@@ -20377,7 +20377,7 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" s="53" t="s">
-        <v>1185</v>
+        <v>1173</v>
       </c>
       <c r="B341" s="32" t="s">
         <v>1104</v>
@@ -20396,7 +20396,7 @@
         <v>1</v>
       </c>
       <c r="H341" s="6" t="s">
-        <v>1208</v>
+        <v>1196</v>
       </c>
       <c r="I341" s="30" t="s">
         <v>1046</v>
@@ -20421,107 +20421,107 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J150:J167 J67:J98 J1:J65 J169:J201 J261 J280 M215 J327 J292:J317 J323 J319 J217:J242 J329:J1048576 J129:J148">
-    <cfRule type="containsText" dxfId="23" priority="42" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="20" priority="42" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66">
-    <cfRule type="containsText" dxfId="21" priority="39" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="19" priority="39" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J243:J260">
-    <cfRule type="containsText" dxfId="20" priority="35" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="18" priority="35" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J262:J279">
-    <cfRule type="containsText" dxfId="19" priority="34" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="17" priority="34" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J262)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J281:J291">
-    <cfRule type="containsText" dxfId="18" priority="33" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J281)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M202:M210">
-    <cfRule type="containsText" dxfId="17" priority="32" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="15" priority="32" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",M202)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M214">
-    <cfRule type="containsText" dxfId="16" priority="30" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="14" priority="30" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",M214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M216">
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="13" priority="26" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",M216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J320">
-    <cfRule type="containsText" dxfId="14" priority="25" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J320)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J321">
-    <cfRule type="containsText" dxfId="13" priority="24" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="11" priority="24" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J321)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J322">
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J322)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J324">
-    <cfRule type="containsText" dxfId="11" priority="22" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="9" priority="22" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J324)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J318">
-    <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J318)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J328">
-    <cfRule type="containsText" dxfId="9" priority="16" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J328)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J325">
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J325)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J326">
-    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J326)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M211:M213">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",M211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J99:J122">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J99)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:J128">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J149">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J168">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",J168)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>